<commit_message>
Fix discontinous id of jlfap file
</commit_message>
<xml_diff>
--- a/Luanvan/Task.xlsx
+++ b/Luanvan/Task.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Lỗ hổng SQL injection</t>
   </si>
@@ -102,6 +102,24 @@
   </si>
   <si>
     <t>Content base</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Out of band</t>
+  </si>
+  <si>
+    <t>Chuong 1</t>
+  </si>
+  <si>
+    <t>Chuong 2</t>
+  </si>
+  <si>
+    <t>Chuong 3</t>
+  </si>
+  <si>
+    <t>Phu luc</t>
   </si>
 </sst>
 </file>
@@ -498,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H20"/>
+  <dimension ref="A2:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,14 +530,17 @@
     <col min="6" max="6" width="30.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2">
         <v>10</v>
       </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
       <c r="E3" t="s">
         <v>24</v>
       </c>
@@ -527,7 +548,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -544,7 +565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -558,7 +579,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -572,7 +593,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -589,7 +610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -602,8 +623,11 @@
       <c r="H8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -617,7 +641,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
@@ -631,7 +655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -645,7 +669,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>17</v>
       </c>
@@ -653,7 +677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>1</v>
       </c>
@@ -661,7 +685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
         <v>19</v>
       </c>
@@ -672,7 +696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>25</v>
       </c>
@@ -680,7 +704,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>18</v>
       </c>
@@ -688,24 +712,50 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>30</v>
+      </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19">
+        <v>30</v>
+      </c>
       <c r="F19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20">
+        <v>30</v>
+      </c>
       <c r="F20" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>